<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@bf6256b31ed9df5aa0cf680f588ae6e81ac45be0 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-adaptor-trimmed-cs.xlsx
+++ b/CodeSystem-adaptor-trimmed-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-12T18:14:21+00:00</t>
+    <t>2024-09-13T20:57:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -114,7 +114,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
   <si>
     <t>Level</t>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -494,6 +500,18 @@
       </c>
       <c r="D3" s="2"/>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@ff860e390131ef809d5db8473ac6aa87de0e2d2d 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-adaptor-trimmed-cs.xlsx
+++ b/CodeSystem-adaptor-trimmed-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-24T15:08:47+00:00</t>
+    <t>2025-05-11T16:39:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@b701e861ff4aea87f49ab6a6b6da8d47ed8dfde7 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-adaptor-trimmed-cs.xlsx
+++ b/CodeSystem-adaptor-trimmed-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Property</t>
   </si>
@@ -48,16 +48,19 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-21T14:22:51+00:00</t>
+    <t>2025-06-13T15:45:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -88,6 +91,9 @@
   </si>
   <si>
     <t>Case Sensitive</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>Value Set (all codes)</t>
@@ -343,43 +349,45 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s" s="2">
         <v>9</v>
@@ -387,66 +395,68 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>26</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -464,51 +474,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2"/>
     </row>

</xml_diff>